<commit_message>
introduced natural gas boiler case
</commit_message>
<xml_diff>
--- a/data/inputs/lci_moeschberg.xlsx
+++ b/data/inputs/lci_moeschberg.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="45">
   <si>
     <t>Database</t>
   </si>
@@ -145,13 +145,22 @@
   </si>
   <si>
     <t>energy demand, operational, Hotel Moeschberg</t>
+  </si>
+  <si>
+    <t>heat supply, Hotel Moeschberg, 2021, natural gas boiler</t>
+  </si>
+  <si>
+    <t>heat production, natural gas, at boiler condensing modulating &lt;100kW</t>
+  </si>
+  <si>
+    <t>heat, central or small-scale, natural gas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +171,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -188,13 +204,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1213,161 +1230,303 @@
         <v>1</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>5</v>
-      </c>
-      <c r="B57" t="str">
-        <f>B54</f>
-        <v>energy demand, operational, Hotel Moeschberg</v>
+        <v>6</v>
+      </c>
+      <c r="B57" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" t="s">
         <v>6</v>
       </c>
-      <c r="B58" t="s">
+      <c r="G60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" t="str">
+        <f>B54</f>
+        <v>heat supply, Hotel Moeschberg, 2021, natural gas boiler</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" ref="C61" si="5">$B$1</f>
+        <v>energy_moeschberg</v>
+      </c>
+      <c r="D61" t="str">
+        <f>B55</f>
+        <v>CH</v>
+      </c>
+      <c r="E61" t="str">
+        <f>B58</f>
+        <v>megajoule</v>
+      </c>
+      <c r="F61" t="s">
+        <v>14</v>
+      </c>
+      <c r="G61" t="str">
+        <f>B56</f>
+        <v>heat, Hotel Moeschberg</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62">
+        <v>4.6680000000000003E-3</v>
+      </c>
+      <c r="C62" t="s">
+        <v>36</v>
+      </c>
+      <c r="D62" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" t="s">
+        <v>23</v>
+      </c>
+      <c r="F62" t="s">
+        <v>15</v>
+      </c>
+      <c r="G62" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B63">
+        <v>0.99529999999999996</v>
+      </c>
+      <c r="C63" t="s">
+        <v>36</v>
+      </c>
+      <c r="D63" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" t="s">
+        <v>23</v>
+      </c>
+      <c r="F63" t="s">
+        <v>15</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" t="str">
+        <f>B65</f>
+        <v>energy demand, operational, Hotel Moeschberg</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>8</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B70" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>11</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B72" t="s">
         <v>12</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C72" t="s">
         <v>13</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D72" t="s">
         <v>4</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E72" t="s">
         <v>8</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F72" t="s">
         <v>6</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G72" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" t="str">
-        <f>B54</f>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" t="str">
+        <f>B65</f>
         <v>energy demand, operational, Hotel Moeschberg</v>
       </c>
-      <c r="B62">
+      <c r="B73">
         <v>1</v>
       </c>
-      <c r="C62" t="str">
-        <f t="shared" ref="C62" si="5">$B$1</f>
+      <c r="C73" t="str">
+        <f t="shared" ref="C73" si="6">$B$1</f>
         <v>energy_moeschberg</v>
       </c>
-      <c r="D62" t="str">
-        <f>B56</f>
+      <c r="D73" t="str">
+        <f>B67</f>
         <v>CH</v>
       </c>
-      <c r="E62" t="str">
-        <f>B59</f>
+      <c r="E73" t="str">
+        <f>B70</f>
         <v>unit</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F73" t="s">
         <v>14</v>
       </c>
-      <c r="G62" t="str">
-        <f>B57</f>
+      <c r="G73" t="str">
+        <f>B68</f>
         <v>energy demand, operational, Hotel Moeschberg</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" t="str">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" t="str">
         <f>A11</f>
         <v>electricity supply, Hotel Moeschberg, 2021</v>
       </c>
-      <c r="B63">
+      <c r="B74">
         <v>32179</v>
       </c>
-      <c r="C63" t="str">
-        <f t="shared" ref="C63:C64" si="6">$B$1</f>
+      <c r="C74" t="str">
+        <f t="shared" ref="C74:C75" si="7">$B$1</f>
         <v>energy_moeschberg</v>
       </c>
-      <c r="D63" t="str">
-        <f t="shared" ref="D63:G63" si="7">D11</f>
+      <c r="D74" t="str">
+        <f t="shared" ref="D74:G74" si="8">D11</f>
         <v>CH</v>
       </c>
-      <c r="E63" t="str">
-        <f t="shared" si="7"/>
+      <c r="E74" t="str">
+        <f t="shared" si="8"/>
         <v>kilowatt hour</v>
       </c>
-      <c r="F63" t="str">
-        <f t="shared" si="7"/>
+      <c r="F74" t="str">
+        <f t="shared" si="8"/>
         <v>production</v>
       </c>
-      <c r="G63" t="str">
-        <f t="shared" si="7"/>
+      <c r="G74" t="str">
+        <f t="shared" si="8"/>
         <v>electricity, low voltage</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" t="str">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" t="str">
         <f>A50</f>
         <v>heat supply, Hotel Moeschberg, 2021</v>
       </c>
-      <c r="B64">
+      <c r="B75">
         <v>655489</v>
       </c>
-      <c r="C64" t="str">
-        <f t="shared" si="6"/>
+      <c r="C75" t="str">
+        <f t="shared" si="7"/>
         <v>energy_moeschberg</v>
       </c>
-      <c r="D64" t="str">
-        <f t="shared" ref="D64:G64" si="8">D50</f>
+      <c r="D75" t="str">
+        <f t="shared" ref="D75:G75" si="9">D50</f>
         <v>CH</v>
       </c>
-      <c r="E64" t="str">
-        <f t="shared" si="8"/>
+      <c r="E75" t="str">
+        <f t="shared" si="9"/>
         <v>megajoule</v>
       </c>
-      <c r="F64" t="str">
-        <f t="shared" si="8"/>
+      <c r="F75" t="str">
+        <f t="shared" si="9"/>
         <v>production</v>
       </c>
-      <c r="G64" t="str">
-        <f t="shared" si="8"/>
+      <c r="G75" t="str">
+        <f t="shared" si="9"/>
         <v>heat, Hotel Moeschberg</v>
       </c>
     </row>

</xml_diff>